<commit_message>
Antes de incluir la seleccion de horario en el OrderViewController
</commit_message>
<xml_diff>
--- a/ToDos.xlsx
+++ b/ToDos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Archivo</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Esta harcodeado para agregar solo 2 Institutos</t>
+  </si>
+  <si>
+    <t>Catch de Error en la autenticacion</t>
   </si>
 </sst>
 </file>
@@ -350,15 +353,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B5"/>
+  <dimension ref="A3:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -377,6 +381,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>